<commit_message>
some progress on poll page and ERD change
</commit_message>
<xml_diff>
--- a/DB_ERD.xlsx
+++ b/DB_ERD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18360" windowHeight="15400" tabRatio="500"/>
+    <workbookView xWindow="3940" yWindow="3160" windowWidth="18360" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>users</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>content</t>
   </si>
   <si>
     <t>create_date</t>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>voter_id (FK)</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>option_id (FK)</t>
   </si>
 </sst>
 </file>
@@ -780,352 +783,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>820615</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>107461</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9769</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>156308</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Freeform 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5802923" y="722923"/>
-          <a:ext cx="1680308" cy="664308"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 1680308 w 1680308"/>
-            <a:gd name="connsiteY0" fmla="*/ 654539 h 664308"/>
-            <a:gd name="connsiteX1" fmla="*/ 1602154 w 1680308"/>
-            <a:gd name="connsiteY1" fmla="*/ 664308 h 664308"/>
-            <a:gd name="connsiteX2" fmla="*/ 1533769 w 1680308"/>
-            <a:gd name="connsiteY2" fmla="*/ 654539 h 664308"/>
-            <a:gd name="connsiteX3" fmla="*/ 1455615 w 1680308"/>
-            <a:gd name="connsiteY3" fmla="*/ 644769 h 664308"/>
-            <a:gd name="connsiteX4" fmla="*/ 1397000 w 1680308"/>
-            <a:gd name="connsiteY4" fmla="*/ 635000 h 664308"/>
-            <a:gd name="connsiteX5" fmla="*/ 1172308 w 1680308"/>
-            <a:gd name="connsiteY5" fmla="*/ 615462 h 664308"/>
-            <a:gd name="connsiteX6" fmla="*/ 1094154 w 1680308"/>
-            <a:gd name="connsiteY6" fmla="*/ 595923 h 664308"/>
-            <a:gd name="connsiteX7" fmla="*/ 1016000 w 1680308"/>
-            <a:gd name="connsiteY7" fmla="*/ 576385 h 664308"/>
-            <a:gd name="connsiteX8" fmla="*/ 986692 w 1680308"/>
-            <a:gd name="connsiteY8" fmla="*/ 556846 h 664308"/>
-            <a:gd name="connsiteX9" fmla="*/ 928077 w 1680308"/>
-            <a:gd name="connsiteY9" fmla="*/ 527539 h 664308"/>
-            <a:gd name="connsiteX10" fmla="*/ 908539 w 1680308"/>
-            <a:gd name="connsiteY10" fmla="*/ 508000 h 664308"/>
-            <a:gd name="connsiteX11" fmla="*/ 879231 w 1680308"/>
-            <a:gd name="connsiteY11" fmla="*/ 488462 h 664308"/>
-            <a:gd name="connsiteX12" fmla="*/ 801077 w 1680308"/>
-            <a:gd name="connsiteY12" fmla="*/ 429846 h 664308"/>
-            <a:gd name="connsiteX13" fmla="*/ 742462 w 1680308"/>
-            <a:gd name="connsiteY13" fmla="*/ 410308 h 664308"/>
-            <a:gd name="connsiteX14" fmla="*/ 713154 w 1680308"/>
-            <a:gd name="connsiteY14" fmla="*/ 400539 h 664308"/>
-            <a:gd name="connsiteX15" fmla="*/ 654539 w 1680308"/>
-            <a:gd name="connsiteY15" fmla="*/ 371231 h 664308"/>
-            <a:gd name="connsiteX16" fmla="*/ 635000 w 1680308"/>
-            <a:gd name="connsiteY16" fmla="*/ 351692 h 664308"/>
-            <a:gd name="connsiteX17" fmla="*/ 576385 w 1680308"/>
-            <a:gd name="connsiteY17" fmla="*/ 322385 h 664308"/>
-            <a:gd name="connsiteX18" fmla="*/ 527539 w 1680308"/>
-            <a:gd name="connsiteY18" fmla="*/ 283308 h 664308"/>
-            <a:gd name="connsiteX19" fmla="*/ 478692 w 1680308"/>
-            <a:gd name="connsiteY19" fmla="*/ 234462 h 664308"/>
-            <a:gd name="connsiteX20" fmla="*/ 459154 w 1680308"/>
-            <a:gd name="connsiteY20" fmla="*/ 214923 h 664308"/>
-            <a:gd name="connsiteX21" fmla="*/ 420077 w 1680308"/>
-            <a:gd name="connsiteY21" fmla="*/ 166077 h 664308"/>
-            <a:gd name="connsiteX22" fmla="*/ 400539 w 1680308"/>
-            <a:gd name="connsiteY22" fmla="*/ 136769 h 664308"/>
-            <a:gd name="connsiteX23" fmla="*/ 361462 w 1680308"/>
-            <a:gd name="connsiteY23" fmla="*/ 97692 h 664308"/>
-            <a:gd name="connsiteX24" fmla="*/ 332154 w 1680308"/>
-            <a:gd name="connsiteY24" fmla="*/ 58615 h 664308"/>
-            <a:gd name="connsiteX25" fmla="*/ 302846 w 1680308"/>
-            <a:gd name="connsiteY25" fmla="*/ 48846 h 664308"/>
-            <a:gd name="connsiteX26" fmla="*/ 273539 w 1680308"/>
-            <a:gd name="connsiteY26" fmla="*/ 29308 h 664308"/>
-            <a:gd name="connsiteX27" fmla="*/ 175846 w 1680308"/>
-            <a:gd name="connsiteY27" fmla="*/ 0 h 664308"/>
-            <a:gd name="connsiteX28" fmla="*/ 0 w 1680308"/>
-            <a:gd name="connsiteY28" fmla="*/ 9769 h 664308"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX5" y="connsiteY5"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX6" y="connsiteY6"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX7" y="connsiteY7"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX8" y="connsiteY8"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX9" y="connsiteY9"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX10" y="connsiteY10"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX11" y="connsiteY11"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX12" y="connsiteY12"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX13" y="connsiteY13"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX14" y="connsiteY14"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX15" y="connsiteY15"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX16" y="connsiteY16"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX17" y="connsiteY17"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX18" y="connsiteY18"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX19" y="connsiteY19"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX20" y="connsiteY20"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX21" y="connsiteY21"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX22" y="connsiteY22"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX23" y="connsiteY23"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX24" y="connsiteY24"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX25" y="connsiteY25"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX26" y="connsiteY26"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX27" y="connsiteY27"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX28" y="connsiteY28"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="1680308" h="664308">
-              <a:moveTo>
-                <a:pt x="1680308" y="654539"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="1654257" y="657795"/>
-                <a:pt x="1628408" y="664308"/>
-                <a:pt x="1602154" y="664308"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="1579128" y="664308"/>
-                <a:pt x="1556593" y="657582"/>
-                <a:pt x="1533769" y="654539"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="1455615" y="644769"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="1436006" y="641968"/>
-                <a:pt x="1416703" y="637038"/>
-                <a:pt x="1397000" y="635000"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="1322219" y="627264"/>
-                <a:pt x="1172308" y="615462"/>
-                <a:pt x="1172308" y="615462"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="1116284" y="596786"/>
-                <a:pt x="1170775" y="613604"/>
-                <a:pt x="1094154" y="595923"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="1067989" y="589885"/>
-                <a:pt x="1016000" y="576385"/>
-                <a:pt x="1016000" y="576385"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="1006231" y="569872"/>
-                <a:pt x="997194" y="562097"/>
-                <a:pt x="986692" y="556846"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="938542" y="532771"/>
-                <a:pt x="974737" y="564868"/>
-                <a:pt x="928077" y="527539"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="920885" y="521785"/>
-                <a:pt x="915731" y="513754"/>
-                <a:pt x="908539" y="508000"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="899371" y="500665"/>
-                <a:pt x="888399" y="495797"/>
-                <a:pt x="879231" y="488462"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="846167" y="462011"/>
-                <a:pt x="859505" y="449322"/>
-                <a:pt x="801077" y="429846"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="742462" y="410308"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="713154" y="400539"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="667652" y="355037"/>
-                <a:pt x="726558" y="407241"/>
-                <a:pt x="654539" y="371231"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="646301" y="367112"/>
-                <a:pt x="642192" y="357446"/>
-                <a:pt x="635000" y="351692"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="607947" y="330050"/>
-                <a:pt x="607339" y="332703"/>
-                <a:pt x="576385" y="322385"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="500210" y="246210"/>
-                <a:pt x="626120" y="369566"/>
-                <a:pt x="527539" y="283308"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="510210" y="268145"/>
-                <a:pt x="494974" y="250744"/>
-                <a:pt x="478692" y="234462"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="459154" y="214923"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="440135" y="157865"/>
-                <a:pt x="464266" y="210266"/>
-                <a:pt x="420077" y="166077"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="411775" y="157775"/>
-                <a:pt x="408180" y="145684"/>
-                <a:pt x="400539" y="136769"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="388551" y="122783"/>
-                <a:pt x="372515" y="112429"/>
-                <a:pt x="361462" y="97692"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="351693" y="84666"/>
-                <a:pt x="344662" y="69038"/>
-                <a:pt x="332154" y="58615"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="324243" y="52023"/>
-                <a:pt x="312615" y="52102"/>
-                <a:pt x="302846" y="48846"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="293077" y="42333"/>
-                <a:pt x="284268" y="34076"/>
-                <a:pt x="273539" y="29308"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="242956" y="15715"/>
-                <a:pt x="208325" y="8120"/>
-                <a:pt x="175846" y="0"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="85489" y="18071"/>
-                <a:pt x="143604" y="9769"/>
-                <a:pt x="0" y="9769"/>
-              </a:cubicBezTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9769</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -1816,6 +1473,824 @@
                 <a:pt x="193717" y="2872708"/>
                 <a:pt x="303902" y="2842846"/>
                 <a:pt x="0" y="2842846"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9770</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>145275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>810846</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Freeform 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3331308" y="1376198"/>
+          <a:ext cx="3292230" cy="2648725"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 3292230"/>
+            <a:gd name="connsiteY0" fmla="*/ 2638956 h 2648725"/>
+            <a:gd name="connsiteX1" fmla="*/ 39077 w 3292230"/>
+            <a:gd name="connsiteY1" fmla="*/ 2648725 h 2648725"/>
+            <a:gd name="connsiteX2" fmla="*/ 205154 w 3292230"/>
+            <a:gd name="connsiteY2" fmla="*/ 2638956 h 2648725"/>
+            <a:gd name="connsiteX3" fmla="*/ 293077 w 3292230"/>
+            <a:gd name="connsiteY3" fmla="*/ 2619417 h 2648725"/>
+            <a:gd name="connsiteX4" fmla="*/ 322384 w 3292230"/>
+            <a:gd name="connsiteY4" fmla="*/ 2609648 h 2648725"/>
+            <a:gd name="connsiteX5" fmla="*/ 429846 w 3292230"/>
+            <a:gd name="connsiteY5" fmla="*/ 2580340 h 2648725"/>
+            <a:gd name="connsiteX6" fmla="*/ 547077 w 3292230"/>
+            <a:gd name="connsiteY6" fmla="*/ 2541264 h 2648725"/>
+            <a:gd name="connsiteX7" fmla="*/ 576384 w 3292230"/>
+            <a:gd name="connsiteY7" fmla="*/ 2531494 h 2648725"/>
+            <a:gd name="connsiteX8" fmla="*/ 605692 w 3292230"/>
+            <a:gd name="connsiteY8" fmla="*/ 2521725 h 2648725"/>
+            <a:gd name="connsiteX9" fmla="*/ 654538 w 3292230"/>
+            <a:gd name="connsiteY9" fmla="*/ 2482648 h 2648725"/>
+            <a:gd name="connsiteX10" fmla="*/ 674077 w 3292230"/>
+            <a:gd name="connsiteY10" fmla="*/ 2463110 h 2648725"/>
+            <a:gd name="connsiteX11" fmla="*/ 732692 w 3292230"/>
+            <a:gd name="connsiteY11" fmla="*/ 2443571 h 2648725"/>
+            <a:gd name="connsiteX12" fmla="*/ 791307 w 3292230"/>
+            <a:gd name="connsiteY12" fmla="*/ 2404494 h 2648725"/>
+            <a:gd name="connsiteX13" fmla="*/ 820615 w 3292230"/>
+            <a:gd name="connsiteY13" fmla="*/ 2384956 h 2648725"/>
+            <a:gd name="connsiteX14" fmla="*/ 889000 w 3292230"/>
+            <a:gd name="connsiteY14" fmla="*/ 2355648 h 2648725"/>
+            <a:gd name="connsiteX15" fmla="*/ 918307 w 3292230"/>
+            <a:gd name="connsiteY15" fmla="*/ 2336110 h 2648725"/>
+            <a:gd name="connsiteX16" fmla="*/ 937846 w 3292230"/>
+            <a:gd name="connsiteY16" fmla="*/ 2316571 h 2648725"/>
+            <a:gd name="connsiteX17" fmla="*/ 1025769 w 3292230"/>
+            <a:gd name="connsiteY17" fmla="*/ 2287264 h 2648725"/>
+            <a:gd name="connsiteX18" fmla="*/ 1055077 w 3292230"/>
+            <a:gd name="connsiteY18" fmla="*/ 2277494 h 2648725"/>
+            <a:gd name="connsiteX19" fmla="*/ 1084384 w 3292230"/>
+            <a:gd name="connsiteY19" fmla="*/ 2267725 h 2648725"/>
+            <a:gd name="connsiteX20" fmla="*/ 1103923 w 3292230"/>
+            <a:gd name="connsiteY20" fmla="*/ 2248187 h 2648725"/>
+            <a:gd name="connsiteX21" fmla="*/ 1162538 w 3292230"/>
+            <a:gd name="connsiteY21" fmla="*/ 2228648 h 2648725"/>
+            <a:gd name="connsiteX22" fmla="*/ 1230923 w 3292230"/>
+            <a:gd name="connsiteY22" fmla="*/ 2170033 h 2648725"/>
+            <a:gd name="connsiteX23" fmla="*/ 1309077 w 3292230"/>
+            <a:gd name="connsiteY23" fmla="*/ 2111417 h 2648725"/>
+            <a:gd name="connsiteX24" fmla="*/ 1348154 w 3292230"/>
+            <a:gd name="connsiteY24" fmla="*/ 2101648 h 2648725"/>
+            <a:gd name="connsiteX25" fmla="*/ 1406769 w 3292230"/>
+            <a:gd name="connsiteY25" fmla="*/ 2062571 h 2648725"/>
+            <a:gd name="connsiteX26" fmla="*/ 1475154 w 3292230"/>
+            <a:gd name="connsiteY26" fmla="*/ 2013725 h 2648725"/>
+            <a:gd name="connsiteX27" fmla="*/ 1494692 w 3292230"/>
+            <a:gd name="connsiteY27" fmla="*/ 1984417 h 2648725"/>
+            <a:gd name="connsiteX28" fmla="*/ 1563077 w 3292230"/>
+            <a:gd name="connsiteY28" fmla="*/ 1925802 h 2648725"/>
+            <a:gd name="connsiteX29" fmla="*/ 1582615 w 3292230"/>
+            <a:gd name="connsiteY29" fmla="*/ 1896494 h 2648725"/>
+            <a:gd name="connsiteX30" fmla="*/ 1592384 w 3292230"/>
+            <a:gd name="connsiteY30" fmla="*/ 1867187 h 2648725"/>
+            <a:gd name="connsiteX31" fmla="*/ 1641230 w 3292230"/>
+            <a:gd name="connsiteY31" fmla="*/ 1828110 h 2648725"/>
+            <a:gd name="connsiteX32" fmla="*/ 1680307 w 3292230"/>
+            <a:gd name="connsiteY32" fmla="*/ 1789033 h 2648725"/>
+            <a:gd name="connsiteX33" fmla="*/ 1699846 w 3292230"/>
+            <a:gd name="connsiteY33" fmla="*/ 1759725 h 2648725"/>
+            <a:gd name="connsiteX34" fmla="*/ 1719384 w 3292230"/>
+            <a:gd name="connsiteY34" fmla="*/ 1720648 h 2648725"/>
+            <a:gd name="connsiteX35" fmla="*/ 1748692 w 3292230"/>
+            <a:gd name="connsiteY35" fmla="*/ 1701110 h 2648725"/>
+            <a:gd name="connsiteX36" fmla="*/ 1758461 w 3292230"/>
+            <a:gd name="connsiteY36" fmla="*/ 1671802 h 2648725"/>
+            <a:gd name="connsiteX37" fmla="*/ 1797538 w 3292230"/>
+            <a:gd name="connsiteY37" fmla="*/ 1613187 h 2648725"/>
+            <a:gd name="connsiteX38" fmla="*/ 1817077 w 3292230"/>
+            <a:gd name="connsiteY38" fmla="*/ 1583879 h 2648725"/>
+            <a:gd name="connsiteX39" fmla="*/ 1836615 w 3292230"/>
+            <a:gd name="connsiteY39" fmla="*/ 1544802 h 2648725"/>
+            <a:gd name="connsiteX40" fmla="*/ 1856154 w 3292230"/>
+            <a:gd name="connsiteY40" fmla="*/ 1525264 h 2648725"/>
+            <a:gd name="connsiteX41" fmla="*/ 1875692 w 3292230"/>
+            <a:gd name="connsiteY41" fmla="*/ 1495956 h 2648725"/>
+            <a:gd name="connsiteX42" fmla="*/ 1895230 w 3292230"/>
+            <a:gd name="connsiteY42" fmla="*/ 1456879 h 2648725"/>
+            <a:gd name="connsiteX43" fmla="*/ 1905000 w 3292230"/>
+            <a:gd name="connsiteY43" fmla="*/ 1427571 h 2648725"/>
+            <a:gd name="connsiteX44" fmla="*/ 1924538 w 3292230"/>
+            <a:gd name="connsiteY44" fmla="*/ 1398264 h 2648725"/>
+            <a:gd name="connsiteX45" fmla="*/ 1953846 w 3292230"/>
+            <a:gd name="connsiteY45" fmla="*/ 1349417 h 2648725"/>
+            <a:gd name="connsiteX46" fmla="*/ 1963615 w 3292230"/>
+            <a:gd name="connsiteY46" fmla="*/ 1320110 h 2648725"/>
+            <a:gd name="connsiteX47" fmla="*/ 1992923 w 3292230"/>
+            <a:gd name="connsiteY47" fmla="*/ 1271264 h 2648725"/>
+            <a:gd name="connsiteX48" fmla="*/ 2032000 w 3292230"/>
+            <a:gd name="connsiteY48" fmla="*/ 1173571 h 2648725"/>
+            <a:gd name="connsiteX49" fmla="*/ 2041769 w 3292230"/>
+            <a:gd name="connsiteY49" fmla="*/ 1144264 h 2648725"/>
+            <a:gd name="connsiteX50" fmla="*/ 2051538 w 3292230"/>
+            <a:gd name="connsiteY50" fmla="*/ 1114956 h 2648725"/>
+            <a:gd name="connsiteX51" fmla="*/ 2080846 w 3292230"/>
+            <a:gd name="connsiteY51" fmla="*/ 1046571 h 2648725"/>
+            <a:gd name="connsiteX52" fmla="*/ 2090615 w 3292230"/>
+            <a:gd name="connsiteY52" fmla="*/ 1007494 h 2648725"/>
+            <a:gd name="connsiteX53" fmla="*/ 2110154 w 3292230"/>
+            <a:gd name="connsiteY53" fmla="*/ 948879 h 2648725"/>
+            <a:gd name="connsiteX54" fmla="*/ 2119923 w 3292230"/>
+            <a:gd name="connsiteY54" fmla="*/ 919571 h 2648725"/>
+            <a:gd name="connsiteX55" fmla="*/ 2129692 w 3292230"/>
+            <a:gd name="connsiteY55" fmla="*/ 890264 h 2648725"/>
+            <a:gd name="connsiteX56" fmla="*/ 2139461 w 3292230"/>
+            <a:gd name="connsiteY56" fmla="*/ 851187 h 2648725"/>
+            <a:gd name="connsiteX57" fmla="*/ 2159000 w 3292230"/>
+            <a:gd name="connsiteY57" fmla="*/ 831648 h 2648725"/>
+            <a:gd name="connsiteX58" fmla="*/ 2198077 w 3292230"/>
+            <a:gd name="connsiteY58" fmla="*/ 724187 h 2648725"/>
+            <a:gd name="connsiteX59" fmla="*/ 2237154 w 3292230"/>
+            <a:gd name="connsiteY59" fmla="*/ 616725 h 2648725"/>
+            <a:gd name="connsiteX60" fmla="*/ 2276230 w 3292230"/>
+            <a:gd name="connsiteY60" fmla="*/ 519033 h 2648725"/>
+            <a:gd name="connsiteX61" fmla="*/ 2286000 w 3292230"/>
+            <a:gd name="connsiteY61" fmla="*/ 489725 h 2648725"/>
+            <a:gd name="connsiteX62" fmla="*/ 2325077 w 3292230"/>
+            <a:gd name="connsiteY62" fmla="*/ 431110 h 2648725"/>
+            <a:gd name="connsiteX63" fmla="*/ 2364154 w 3292230"/>
+            <a:gd name="connsiteY63" fmla="*/ 352956 h 2648725"/>
+            <a:gd name="connsiteX64" fmla="*/ 2373923 w 3292230"/>
+            <a:gd name="connsiteY64" fmla="*/ 323648 h 2648725"/>
+            <a:gd name="connsiteX65" fmla="*/ 2413000 w 3292230"/>
+            <a:gd name="connsiteY65" fmla="*/ 265033 h 2648725"/>
+            <a:gd name="connsiteX66" fmla="*/ 2452077 w 3292230"/>
+            <a:gd name="connsiteY66" fmla="*/ 196648 h 2648725"/>
+            <a:gd name="connsiteX67" fmla="*/ 2481384 w 3292230"/>
+            <a:gd name="connsiteY67" fmla="*/ 177110 h 2648725"/>
+            <a:gd name="connsiteX68" fmla="*/ 2500923 w 3292230"/>
+            <a:gd name="connsiteY68" fmla="*/ 157571 h 2648725"/>
+            <a:gd name="connsiteX69" fmla="*/ 2559538 w 3292230"/>
+            <a:gd name="connsiteY69" fmla="*/ 118494 h 2648725"/>
+            <a:gd name="connsiteX70" fmla="*/ 2588846 w 3292230"/>
+            <a:gd name="connsiteY70" fmla="*/ 98956 h 2648725"/>
+            <a:gd name="connsiteX71" fmla="*/ 2637692 w 3292230"/>
+            <a:gd name="connsiteY71" fmla="*/ 69648 h 2648725"/>
+            <a:gd name="connsiteX72" fmla="*/ 2764692 w 3292230"/>
+            <a:gd name="connsiteY72" fmla="*/ 59879 h 2648725"/>
+            <a:gd name="connsiteX73" fmla="*/ 2813538 w 3292230"/>
+            <a:gd name="connsiteY73" fmla="*/ 50110 h 2648725"/>
+            <a:gd name="connsiteX74" fmla="*/ 2911230 w 3292230"/>
+            <a:gd name="connsiteY74" fmla="*/ 20802 h 2648725"/>
+            <a:gd name="connsiteX75" fmla="*/ 3087077 w 3292230"/>
+            <a:gd name="connsiteY75" fmla="*/ 11033 h 2648725"/>
+            <a:gd name="connsiteX76" fmla="*/ 3292230 w 3292230"/>
+            <a:gd name="connsiteY76" fmla="*/ 1264 h 2648725"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX25" y="connsiteY25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX26" y="connsiteY26"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX27" y="connsiteY27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX28" y="connsiteY28"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX29" y="connsiteY29"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX30" y="connsiteY30"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX31" y="connsiteY31"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX32" y="connsiteY32"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX33" y="connsiteY33"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX34" y="connsiteY34"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX35" y="connsiteY35"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX36" y="connsiteY36"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX37" y="connsiteY37"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX38" y="connsiteY38"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX39" y="connsiteY39"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX40" y="connsiteY40"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX41" y="connsiteY41"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX42" y="connsiteY42"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX43" y="connsiteY43"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX44" y="connsiteY44"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX45" y="connsiteY45"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX46" y="connsiteY46"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX47" y="connsiteY47"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX48" y="connsiteY48"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX49" y="connsiteY49"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX50" y="connsiteY50"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX51" y="connsiteY51"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX52" y="connsiteY52"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX53" y="connsiteY53"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX54" y="connsiteY54"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX55" y="connsiteY55"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX56" y="connsiteY56"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX57" y="connsiteY57"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX58" y="connsiteY58"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX59" y="connsiteY59"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX60" y="connsiteY60"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX61" y="connsiteY61"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX62" y="connsiteY62"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX63" y="connsiteY63"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX64" y="connsiteY64"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX65" y="connsiteY65"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX66" y="connsiteY66"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX67" y="connsiteY67"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX68" y="connsiteY68"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX69" y="connsiteY69"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX70" y="connsiteY70"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX71" y="connsiteY71"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX72" y="connsiteY72"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX73" y="connsiteY73"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX74" y="connsiteY74"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX75" y="connsiteY75"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX76" y="connsiteY76"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="3292230" h="2648725">
+              <a:moveTo>
+                <a:pt x="0" y="2638956"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="13026" y="2642212"/>
+                <a:pt x="25650" y="2648725"/>
+                <a:pt x="39077" y="2648725"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="94532" y="2648725"/>
+                <a:pt x="149927" y="2643977"/>
+                <a:pt x="205154" y="2638956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="219934" y="2637612"/>
+                <a:pt x="276084" y="2624272"/>
+                <a:pt x="293077" y="2619417"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="302978" y="2616588"/>
+                <a:pt x="312394" y="2612145"/>
+                <a:pt x="322384" y="2609648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="432854" y="2582031"/>
+                <a:pt x="304091" y="2622258"/>
+                <a:pt x="429846" y="2580340"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="547077" y="2541264"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="576384" y="2531494"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="605692" y="2521725"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="644604" y="2463355"/>
+                <a:pt x="602109" y="2514104"/>
+                <a:pt x="654538" y="2482648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="662436" y="2477909"/>
+                <a:pt x="665839" y="2467229"/>
+                <a:pt x="674077" y="2463110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="692498" y="2453900"/>
+                <a:pt x="732692" y="2443571"/>
+                <a:pt x="732692" y="2443571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="788248" y="2388017"/>
+                <a:pt x="734757" y="2432770"/>
+                <a:pt x="791307" y="2404494"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="801809" y="2399243"/>
+                <a:pt x="810421" y="2390781"/>
+                <a:pt x="820615" y="2384956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="854420" y="2365639"/>
+                <a:pt x="856117" y="2366609"/>
+                <a:pt x="889000" y="2355648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="898769" y="2349135"/>
+                <a:pt x="909139" y="2343444"/>
+                <a:pt x="918307" y="2336110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="925499" y="2330356"/>
+                <a:pt x="929608" y="2320690"/>
+                <a:pt x="937846" y="2316571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="937851" y="2316568"/>
+                <a:pt x="1011113" y="2292150"/>
+                <a:pt x="1025769" y="2287264"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1055077" y="2277494"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1084384" y="2267725"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1090897" y="2261212"/>
+                <a:pt x="1095685" y="2252306"/>
+                <a:pt x="1103923" y="2248187"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1122344" y="2238977"/>
+                <a:pt x="1162538" y="2228648"/>
+                <a:pt x="1162538" y="2228648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1256614" y="2134572"/>
+                <a:pt x="1156524" y="2229552"/>
+                <a:pt x="1230923" y="2170033"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1260516" y="2146358"/>
+                <a:pt x="1259494" y="2123813"/>
+                <a:pt x="1309077" y="2111417"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="1348154" y="2101648"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="1367692" y="2088622"/>
+                <a:pt x="1387983" y="2076660"/>
+                <a:pt x="1406769" y="2062571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1455239" y="2026219"/>
+                <a:pt x="1432299" y="2042296"/>
+                <a:pt x="1475154" y="2013725"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1481667" y="2003956"/>
+                <a:pt x="1486390" y="1992719"/>
+                <a:pt x="1494692" y="1984417"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1538885" y="1940224"/>
+                <a:pt x="1516392" y="1995832"/>
+                <a:pt x="1563077" y="1925802"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1569590" y="1916033"/>
+                <a:pt x="1577364" y="1906996"/>
+                <a:pt x="1582615" y="1896494"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1587220" y="1887284"/>
+                <a:pt x="1587086" y="1876017"/>
+                <a:pt x="1592384" y="1867187"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1604122" y="1847624"/>
+                <a:pt x="1624786" y="1842205"/>
+                <a:pt x="1641230" y="1828110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1655216" y="1816122"/>
+                <a:pt x="1668319" y="1803019"/>
+                <a:pt x="1680307" y="1789033"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1687948" y="1780118"/>
+                <a:pt x="1694021" y="1769919"/>
+                <a:pt x="1699846" y="1759725"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1707071" y="1747081"/>
+                <a:pt x="1710061" y="1731836"/>
+                <a:pt x="1719384" y="1720648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1726901" y="1711628"/>
+                <a:pt x="1738923" y="1707623"/>
+                <a:pt x="1748692" y="1701110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1751948" y="1691341"/>
+                <a:pt x="1753460" y="1680804"/>
+                <a:pt x="1758461" y="1671802"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1769865" y="1651275"/>
+                <a:pt x="1784512" y="1632725"/>
+                <a:pt x="1797538" y="1613187"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1804051" y="1603418"/>
+                <a:pt x="1811826" y="1594381"/>
+                <a:pt x="1817077" y="1583879"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1823590" y="1570853"/>
+                <a:pt x="1828537" y="1556919"/>
+                <a:pt x="1836615" y="1544802"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1841724" y="1537138"/>
+                <a:pt x="1850400" y="1532456"/>
+                <a:pt x="1856154" y="1525264"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1863489" y="1516096"/>
+                <a:pt x="1869867" y="1506150"/>
+                <a:pt x="1875692" y="1495956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1882917" y="1483312"/>
+                <a:pt x="1889493" y="1470265"/>
+                <a:pt x="1895230" y="1456879"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1899287" y="1447414"/>
+                <a:pt x="1900395" y="1436782"/>
+                <a:pt x="1905000" y="1427571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1910251" y="1417070"/>
+                <a:pt x="1918025" y="1408033"/>
+                <a:pt x="1924538" y="1398264"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1952211" y="1315243"/>
+                <a:pt x="1913617" y="1416465"/>
+                <a:pt x="1953846" y="1349417"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1959144" y="1340587"/>
+                <a:pt x="1959010" y="1329320"/>
+                <a:pt x="1963615" y="1320110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1972107" y="1303127"/>
+                <a:pt x="1983702" y="1287862"/>
+                <a:pt x="1992923" y="1271264"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2016879" y="1228144"/>
+                <a:pt x="2014634" y="1225668"/>
+                <a:pt x="2032000" y="1173571"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="2041769" y="1144264"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="2045025" y="1134495"/>
+                <a:pt x="2046933" y="1124167"/>
+                <a:pt x="2051538" y="1114956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2068907" y="1080219"/>
+                <a:pt x="2071263" y="1080113"/>
+                <a:pt x="2080846" y="1046571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2084534" y="1033661"/>
+                <a:pt x="2086757" y="1020354"/>
+                <a:pt x="2090615" y="1007494"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2096533" y="987767"/>
+                <a:pt x="2103641" y="968417"/>
+                <a:pt x="2110154" y="948879"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="2119923" y="919571"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="2123179" y="909802"/>
+                <a:pt x="2127195" y="900254"/>
+                <a:pt x="2129692" y="890264"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2132948" y="877238"/>
+                <a:pt x="2133456" y="863196"/>
+                <a:pt x="2139461" y="851187"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2143580" y="842949"/>
+                <a:pt x="2152487" y="838161"/>
+                <a:pt x="2159000" y="831648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2171945" y="799284"/>
+                <a:pt x="2189718" y="757623"/>
+                <a:pt x="2198077" y="724187"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2220463" y="634642"/>
+                <a:pt x="2202719" y="668376"/>
+                <a:pt x="2237154" y="616725"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2281619" y="483326"/>
+                <a:pt x="2233112" y="619642"/>
+                <a:pt x="2276230" y="519033"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2280287" y="509568"/>
+                <a:pt x="2280999" y="498727"/>
+                <a:pt x="2286000" y="489725"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2297404" y="469198"/>
+                <a:pt x="2325077" y="431110"/>
+                <a:pt x="2325077" y="431110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2347528" y="363756"/>
+                <a:pt x="2330051" y="387057"/>
+                <a:pt x="2364154" y="352956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2367410" y="343187"/>
+                <a:pt x="2368922" y="332650"/>
+                <a:pt x="2373923" y="323648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2385327" y="303121"/>
+                <a:pt x="2413000" y="265033"/>
+                <a:pt x="2413000" y="265033"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2424177" y="231500"/>
+                <a:pt x="2422504" y="226221"/>
+                <a:pt x="2452077" y="196648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2460379" y="188346"/>
+                <a:pt x="2472216" y="184444"/>
+                <a:pt x="2481384" y="177110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2488576" y="171356"/>
+                <a:pt x="2493554" y="163097"/>
+                <a:pt x="2500923" y="157571"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2519709" y="143482"/>
+                <a:pt x="2540000" y="131520"/>
+                <a:pt x="2559538" y="118494"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2569307" y="111981"/>
+                <a:pt x="2580544" y="107258"/>
+                <a:pt x="2588846" y="98956"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2607564" y="80237"/>
+                <a:pt x="2608704" y="73271"/>
+                <a:pt x="2637692" y="69648"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2679823" y="64382"/>
+                <a:pt x="2722359" y="63135"/>
+                <a:pt x="2764692" y="59879"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2780974" y="56623"/>
+                <a:pt x="2797519" y="54479"/>
+                <a:pt x="2813538" y="50110"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2829409" y="45781"/>
+                <a:pt x="2888342" y="22883"/>
+                <a:pt x="2911230" y="20802"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2969695" y="15487"/>
+                <a:pt x="3028461" y="14289"/>
+                <a:pt x="3087077" y="11033"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3200592" y="-5183"/>
+                <a:pt x="3132435" y="1264"/>
+                <a:pt x="3292230" y="1264"/>
               </a:cubicBezTo>
             </a:path>
           </a:pathLst>
@@ -2118,7 +2593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2133,7 +2610,7 @@
         <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -2155,7 +2632,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
@@ -2166,7 +2643,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
@@ -2177,7 +2654,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -2185,35 +2662,35 @@
         <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.2">
@@ -2226,7 +2703,7 @@
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>4</v>
@@ -2234,7 +2711,7 @@
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>5</v>
@@ -2247,6 +2724,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>